<commit_message>
Actualización completa del proyecto
</commit_message>
<xml_diff>
--- a/documentacion/bitacora_proyecto.xlsx
+++ b/documentacion/bitacora_proyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\FlutterProjects\FWS_Dashboard_Produccion\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C102888D-9864-4626-9513-0125C5422BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2733F1-6141-4E57-9951-9B28D91F2A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -290,7 +290,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="16">
     <dxf>
       <font>
         <b/>
@@ -358,84 +358,7 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -495,17 +418,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{46C1A9BA-57C8-4F7C-9401-F089B917CE5E}" name="Tabla1" displayName="Tabla1" ref="A1:H7" totalsRowShown="0" headerRowDxfId="14" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{46C1A9BA-57C8-4F7C-9401-F089B917CE5E}" name="Tabla1" displayName="Tabla1" ref="A1:H7" totalsRowShown="0" headerRowDxfId="7" dataDxfId="8">
   <autoFilter ref="A1:H7" xr:uid="{46C1A9BA-57C8-4F7C-9401-F089B917CE5E}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{EE3BC860-FA8E-45B7-A0CF-5779F14D795C}" name="ID" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{C08DDA40-606A-4A70-B160-3505FEC5EE0D}" name="Fecha" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{AA311DEF-8C76-4919-A541-75906CD9907A}" name="Módulo / Área" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{414A2CEF-731B-4613-A59C-14A7A164D579}" name="Descripción de la Actividad / Cambio" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{B0E39B7D-6DB4-432C-90AC-4EB4B45DD4CF}" name="Responsable" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{A1A3A4BC-BC85-4BCC-B66F-1063FB9747FA}" name="Estado" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{F41A7471-2DA6-47A9-A97D-3323E7DC823C}" name="Prioridad" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{5E1B98B9-1CAC-48EE-A9DF-634F34419054}" name="Notas / Observaciones" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{EE3BC860-FA8E-45B7-A0CF-5779F14D795C}" name="ID" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{C08DDA40-606A-4A70-B160-3505FEC5EE0D}" name="Fecha" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{AA311DEF-8C76-4919-A541-75906CD9907A}" name="Módulo / Área" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{414A2CEF-731B-4613-A59C-14A7A164D579}" name="Descripción de la Actividad / Cambio" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{B0E39B7D-6DB4-432C-90AC-4EB4B45DD4CF}" name="Responsable" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{A1A3A4BC-BC85-4BCC-B66F-1063FB9747FA}" name="Estado" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{F41A7471-2DA6-47A9-A97D-3323E7DC823C}" name="Prioridad" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{5E1B98B9-1CAC-48EE-A9DF-634F34419054}" name="Notas / Observaciones" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -777,7 +700,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -976,24 +899,24 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F7">
-    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="✅ Finalizado">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="✅ Finalizado">
       <formula>NOT(ISERROR(SEARCH("✅ Finalizado",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="⏳ En proceso">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="⏳ En proceso">
       <formula>NOT(ISERROR(SEARCH("⏳ En proceso",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="4" operator="containsText" text="❌ Detenido / Cancelado">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="❌ Detenido / Cancelado">
       <formula>NOT(ISERROR(SEARCH("❌ Detenido / Cancelado",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G7">
-    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="Alta">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Alta">
       <formula>NOT(ISERROR(SEARCH("Alta",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="Media">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Media">
       <formula>NOT(ISERROR(SEARCH("Media",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Baja">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Baja">
       <formula>NOT(ISERROR(SEARCH("Baja",G2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>